<commit_message>
Insert Image in Excel
</commit_message>
<xml_diff>
--- a/NewsRanking_2024_04_25_목.xlsx
+++ b/NewsRanking_2024_04_25_목.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>No.</t>
   </si>
@@ -26,61 +26,121 @@
     <t>[속보] 민주당 "영수회담 일정 논의 불발"</t>
   </si>
   <si>
+    <t>./images/image_1.png</t>
+  </si>
+  <si>
     <t>김재섭에 '험지 당선' 비결 물으니… "국힘 반대로만 했다"</t>
   </si>
   <si>
+    <t>./images/image_2.png</t>
+  </si>
+  <si>
     <t>이준석 "내가 尹보다 잘할 듯…한동훈은 일단 쉬고 역량 키워야"</t>
   </si>
   <si>
+    <t>./images/image_3.png</t>
+  </si>
+  <si>
     <t>정부 "2026학년도 의대 증원 재논의 조건은 '의료계 통일안'"</t>
   </si>
   <si>
+    <t>./images/image_4.png</t>
+  </si>
+  <si>
     <t>민희진 "하이브가 날 배신… 경영권 찬탈 시도 없어"</t>
   </si>
   <si>
+    <t>./images/image_5.png</t>
+  </si>
+  <si>
     <t>'구하라법' 드디어 빛 본다… 헌재 '유류분 제도' 위헌 판결</t>
   </si>
   <si>
+    <t>./images/image_6.png</t>
+  </si>
+  <si>
     <t>대전 둔산, 청주 용암 등 도시정비 속도 붙는다</t>
   </si>
   <si>
+    <t>./images/image_7.png</t>
+  </si>
+  <si>
     <t>천하람 "尹, 이준석보다 한동훈 더 보기 싫을 것…불쾌·배신감"</t>
   </si>
   <si>
+    <t>./images/image_8.png</t>
+  </si>
+  <si>
     <t>대통령실 "올해 경제성장 당초 2.2% 넘어설 것" 전망</t>
   </si>
   <si>
+    <t>./images/image_9.png</t>
+  </si>
+  <si>
     <t>"순두부라떼, 맛있쥬?" 백종원 손 거친 메뉴, 당진서 맛 본다</t>
   </si>
   <si>
+    <t>./images/image_10.png</t>
+  </si>
+  <si>
     <t>아산·대전서 발견된 유해 2구… 74년 만에 만난 아버지 유골</t>
   </si>
   <si>
+    <t>./images/image_11.png</t>
+  </si>
+  <si>
     <t>대통령실 "영수 회담, 의제 제한 없이 가능한 빨리 개최하자"</t>
   </si>
   <si>
+    <t>./images/image_12.png</t>
+  </si>
+  <si>
     <t>의협 "'무책임한 교수' 발언한 박민수 복지차관 즉각 사퇴해야"</t>
   </si>
   <si>
+    <t>./images/image_13.png</t>
+  </si>
+  <si>
     <t>박지원, 한동훈에 "잘 가시라"… 홍준표엔 "정치력 인정"</t>
   </si>
   <si>
+    <t>./images/image_14.png</t>
+  </si>
+  <si>
     <t>세종 중심상업지 '불법 숙박' 의심업소 31곳 적발...미신고 영업 6명 검찰 송치</t>
   </si>
   <si>
+    <t>./images/image_15.png</t>
+  </si>
+  <si>
     <t>정부 "의대증원 1년 유예? 선택할 수 없는 대안… 집단 사직 '유감'"</t>
   </si>
   <si>
+    <t>./images/image_16.png</t>
+  </si>
+  <si>
     <t>與, 보름 만에 패인 분석 토론…"충청권이 원내1당 결정, 지역 연구 집중해야"</t>
   </si>
   <si>
+    <t>./images/image_17.png</t>
+  </si>
+  <si>
     <t>'화재 3개월 만' 서천특화시장, 임시로 문 열었다</t>
   </si>
   <si>
+    <t>./images/image_18.png</t>
+  </si>
+  <si>
     <t>천안교도소 교도관, 수감자 금품수수 혐의로 검찰 수사</t>
   </si>
   <si>
+    <t>./images/image_19.png</t>
+  </si>
+  <si>
     <t>더민주연합 당선자 4명 원소속 복귀… 10명은 민주당 합류</t>
+  </si>
+  <si>
+    <t>./images/image_20.png</t>
   </si>
 </sst>
 </file>
@@ -149,178 +209,218 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2"/>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3"/>
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4"/>
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5"/>
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6"/>
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7"/>
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>7.0</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8"/>
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>8.0</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9"/>
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>9.0</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10"/>
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>10.0</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11"/>
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>11.0</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12"/>
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12.0</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13"/>
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>13.0</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14"/>
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14.0</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15"/>
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15.0</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16"/>
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>16.0</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17"/>
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>17.0</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18"/>
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18.0</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19"/>
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19.0</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20"/>
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>20.0</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21"/>
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>